<commit_message>
item table update markdown syntax example to parsedown
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/all_widgets.xlsx
+++ b/webroot/assets/example_surveys/all_widgets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25040" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -615,16 +615,16 @@
 A standard format for economising space in paper-pencil, value for online studies doubtful?</t>
   </si>
   <si>
+    <t>range_ticks 1,7,1</t>
+  </si>
+  <si>
     <t>## note
 This note will only appear once, because notes that are followed by further notes or submission buttons are hidden after being displayed once.
 #### by the way
-In Excel you can make linebreaks using Strg+Enter (Windows) or Alt+Apple+Enter (Mac).
-In the `label` column you can use HTML und [Markdown](http://daringfireball.net/projects/markdown/syntax) and `knitr`. A line break in markdown is a little different: The line before the break has to end with two spaces.  
-You can start a new paragraph using a blank line.
+In Excel you can make linebreaks using Strg+Enter (Windows) or Alt+Apple+Enter (Mac). 
+You can start a new paragraph by using a blank line.
+In the `label` column you can use HTML und [Markdown](http://daringfireball.net/projects/markdown/syntax) and `knitr`.
 Make text __bold__ through  `__bold__`, make it *italic* through `*italic*`.</t>
-  </si>
-  <si>
-    <t>range_ticks 1,7,1</t>
   </si>
 </sst>
 </file>
@@ -1083,8 +1083,8 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1139,7 +1139,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="255">
+    <row r="2" spans="1:12" ht="225">
       <c r="C2" s="8" t="s">
         <v>151</v>
       </c>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
@@ -1357,7 +1357,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
update docs to reflect new char limits
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/all_widgets.xlsx
+++ b/webroot/assets/example_surveys/all_widgets.xlsx
@@ -109,9 +109,6 @@
     <t>eigenschaften</t>
   </si>
   <si>
-    <t>onlyonce</t>
-  </si>
-  <si>
     <t>confirm1</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
 You can start a new paragraph by using a blank line.
 In the `label` column you can use HTML und [Markdown](http://daringfireball.net/projects/markdown/syntax) and `knitr`.
 Make text __bold__ through  `__bold__`, make it *italic* through `*italic*`.</t>
+  </si>
+  <si>
+    <t>note_shown_only_once</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1084,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1103,64 +1103,64 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="18">
       <c r="A1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="H1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="C2" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>28</v>
+        <v>184</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="C3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1171,29 +1171,29 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="90">
@@ -1204,11 +1204,11 @@
         <v>0</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>22</v>
@@ -1222,20 +1222,20 @@
         <v>9</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="105">
@@ -1243,41 +1243,41 @@
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60">
       <c r="C10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="75">
@@ -1292,13 +1292,13 @@
       </c>
       <c r="E11" s="3"/>
       <c r="G11" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75">
@@ -1310,22 +1310,22 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="180">
       <c r="C13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E13" s="3"/>
       <c r="G13" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1333,89 +1333,89 @@
     </row>
     <row r="15" spans="1:12" ht="135">
       <c r="B15" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="B16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="3"/>
       <c r="G16" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30">
       <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="3"/>
       <c r="G17" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="C18" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="3"/>
       <c r="G18" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="45">
       <c r="C19" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="3"/>
       <c r="G19" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>15</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1442,55 +1442,55 @@
       </c>
       <c r="E21" s="3"/>
       <c r="G21" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30">
       <c r="C22" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="3"/>
       <c r="G22" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30">
       <c r="C23" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="3"/>
       <c r="G23" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H23" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45">
       <c r="C24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="3"/>
       <c r="G24" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1508,26 +1508,26 @@
     </row>
     <row r="28" spans="1:10" ht="30">
       <c r="C28" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="3"/>
       <c r="G28" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="45">
       <c r="C29" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="3"/>
       <c r="G29" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1541,66 +1541,66 @@
         <v>20</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="C32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="C34" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="C35" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1608,58 +1608,58 @@
     </row>
     <row r="37" spans="1:8" ht="45">
       <c r="A37" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:8" ht="75">
       <c r="C38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="E38" s="3"/>
       <c r="G38" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30">
       <c r="C39" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="3"/>
       <c r="G39" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="C40" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="E40" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="C41" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E41" s="3"/>
       <c r="G41" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1667,50 +1667,50 @@
     </row>
     <row r="43" spans="1:8" ht="45">
       <c r="C43" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="3"/>
       <c r="G43" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30">
       <c r="C44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="E44" s="3"/>
       <c r="G44" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="C45" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="E45" s="3"/>
       <c r="G45" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="45">
       <c r="C46" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E46" s="3"/>
       <c r="G46" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1718,32 +1718,32 @@
     </row>
     <row r="48" spans="1:8" ht="45">
       <c r="C48" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" s="3"/>
       <c r="G48" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="45">
       <c r="C49" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E49" s="3"/>
       <c r="G49" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="2:12">
@@ -1758,15 +1758,15 @@
     <row r="53" spans="2:12" ht="30">
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -1776,95 +1776,95 @@
     </row>
     <row r="54" spans="2:12" ht="60">
       <c r="B54" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H54" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J54" s="3" t="s">
+      <c r="K54" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="45">
       <c r="B55" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H55" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="J55" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="K55" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K55" s="3" t="s">
+      <c r="L55" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="56" spans="2:12" ht="45">
       <c r="B56" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="I56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="J56" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J56" s="3" t="s">
+      <c r="K56" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="L56" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="57" spans="2:12">
@@ -1875,28 +1875,28 @@
     </row>
     <row r="59" spans="2:12">
       <c r="C59" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E59" s="3"/>
       <c r="G59" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="2:12" ht="195">
       <c r="C60" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1927,19 +1927,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1990,21 +1990,21 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated schema and code to allow longer names
</commit_message>
<xml_diff>
--- a/webroot/assets/example_surveys/all_widgets.xlsx
+++ b/webroot/assets/example_surveys/all_widgets.xlsx
@@ -11,7 +11,7 @@
     <sheet name="choices" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$G$43:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$G$42:$G$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,14 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="184">
   <si>
     <t>mc</t>
   </si>
   <si>
-    <t>multiplechoice_many</t>
-  </si>
-  <si>
     <t>cool</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>freakig</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
     <t>nix</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
   </si>
   <si>
     <t>slider_list</t>
-  </si>
-  <si>
-    <t>slider_list2</t>
   </si>
   <si>
     <t>left500</t>
@@ -344,9 +335,6 @@
     <t>yourstory</t>
   </si>
   <si>
-    <t>beginning</t>
-  </si>
-  <si>
     <t>abode</t>
   </si>
   <si>
@@ -354,19 +342,12 @@
 Where do you live?</t>
   </si>
   <si>
-    <t>religion</t>
-  </si>
-  <si>
     <t>### MC
 &lt;sup title="If you can't make up your mind, you probably want to click Cthulhu." class="hastooltip"&gt;&lt;i class="icon-circle-blank"&gt;&lt;/i&gt;&lt;/sup&gt;  A simple multiple-choice question with two choices (and a hint).</t>
   </si>
   <si>
     <t>### MC
 A multiple-choice/radio button question with more choices. We can give more spaces to the choices by specifying a [CSS](http://reference.sitepoint.com/css) class in the `class` column.</t>
-  </si>
-  <si>
-    <t>### MC
-If you leave all but the first and the last choices text fields empty, the first choice is automatically placed to the left rather than to the right of its radio button.</t>
   </si>
   <si>
     <t>### Email addresses are automatically checked in newer browsers
@@ -625,6 +606,21 @@
   </si>
   <si>
     <t>note_shown_only_once</t>
+  </si>
+  <si>
+    <t>note_for_items_to_follow</t>
+  </si>
+  <si>
+    <t>multiplechoice_several</t>
+  </si>
+  <si>
+    <t>mc_religion</t>
+  </si>
+  <si>
+    <t>your_email</t>
+  </si>
+  <si>
+    <t>slider_list_longer</t>
   </si>
 </sst>
 </file>
@@ -1080,11 +1076,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1103,476 +1099,469 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="18">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="C2" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="C3" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
       <c r="E3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="B6" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="90">
       <c r="A7" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>181</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="90">
       <c r="A8" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="105">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60">
       <c r="C10" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="75">
+      <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="180">
+      <c r="C12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="G12" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="135">
+      <c r="B14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="G14" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="75">
-      <c r="A11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="G11" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="75">
-      <c r="C12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="180">
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="G13" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="135">
+      <c r="H14" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>39</v>
+        <v>183</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="8" t="s">
-        <v>164</v>
+        <v>109</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>182</v>
+        <v>35</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3"/>
       <c r="G16" s="8" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30">
-      <c r="B17" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3"/>
       <c r="G17" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45">
       <c r="C18" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="3"/>
       <c r="G18" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45">
-      <c r="C19" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="J18" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="G19" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="10" t="s">
-        <v>38</v>
+    </row>
+    <row r="20" spans="1:10" ht="45">
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="45">
+      <c r="G20" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30">
       <c r="C21" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="E21" s="3"/>
       <c r="G21" s="8" t="s">
-        <v>124</v>
+        <v>170</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30">
       <c r="C22" s="8" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="3"/>
       <c r="G22" s="8" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45">
       <c r="C23" s="8" t="s">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="3"/>
       <c r="G23" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45">
-      <c r="C24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>28</v>
-      </c>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="E24" s="3"/>
-      <c r="G24" s="8" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="33">
+      <c r="A26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="12"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="33">
-      <c r="A27" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="12"/>
+    <row r="27" spans="1:10" ht="30">
+      <c r="C27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" ht="30">
+      <c r="G27" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45">
       <c r="C28" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3"/>
       <c r="G28" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="45">
-      <c r="C29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="E29" s="3"/>
-      <c r="G29" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" ht="30">
+    </row>
+    <row r="30" spans="1:10" ht="30">
+      <c r="C30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="C31" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="C32" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1580,171 +1569,160 @@
         <v>49</v>
       </c>
       <c r="D34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="C35" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" ht="45">
+      <c r="A36" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="45">
-      <c r="A37" s="8" t="s">
-        <v>72</v>
+    <row r="37" spans="1:8" ht="75">
+      <c r="C37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" ht="75">
+      <c r="G37" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30">
       <c r="C38" s="8" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E38" s="3"/>
       <c r="G38" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="C39" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="G39" s="8" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="C40" s="8" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E40" s="3"/>
       <c r="G40" s="8" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="C41" s="8" t="s">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="45">
+      <c r="C42" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="G42" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30">
+      <c r="C43" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="G41" s="8" t="s">
+      <c r="D43" s="8" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" ht="45">
-      <c r="C43" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="E43" s="3"/>
       <c r="G43" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="30">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="C44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="E44" s="3"/>
       <c r="G44" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45">
       <c r="C45" s="8" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="E45" s="3"/>
       <c r="G45" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="45">
-      <c r="C46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>94</v>
-      </c>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="E46" s="3"/>
-      <c r="G46" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+    </row>
+    <row r="47" spans="1:8" ht="45">
+      <c r="C47" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="E47" s="3"/>
+      <c r="G47" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="45">
       <c r="C48" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E48" s="3"/>
       <c r="G48" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" ht="45">
-      <c r="C49" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
       <c r="E49" s="3"/>
-      <c r="G49" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="50" spans="2:12">
       <c r="E50" s="3"/>
@@ -1752,155 +1730,152 @@
     <row r="51" spans="2:12">
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" ht="30">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="2:12" ht="30">
-      <c r="B53" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+    </row>
+    <row r="53" spans="2:12" ht="60">
+      <c r="B53" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="C53" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="4" t="s">
+      <c r="G53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K53" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-    </row>
-    <row r="54" spans="2:12" ht="60">
+      <c r="L53" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="45">
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="45">
       <c r="B55" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L55" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" ht="45">
-      <c r="B56" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>99</v>
-      </c>
+    </row>
+    <row r="56" spans="2:12">
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="57" spans="2:12">
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="2:12">
+      <c r="C58" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="2:12">
+      <c r="G58" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="195">
       <c r="C59" s="8" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E59" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="G59" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" ht="195">
-      <c r="C60" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G43:G46"/>
+  <autoFilter ref="G42:G45"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1927,25 +1902,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1953,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1961,7 +1936,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1969,7 +1944,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1977,7 +1952,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1985,26 +1960,26 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>